<commit_message>
Fully Implemented Import EXCEL File
</commit_message>
<xml_diff>
--- a/EzanaLMSData/XLSFiles/ezanaLMS_Lecturers.xlsx
+++ b/EzanaLMSData/XLSFiles/ezanaLMS_Lecturers.xlsx
@@ -20,7 +20,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="169">
+  <si>
+    <t xml:space="preserve">093d69fd815225919ef1a4911c3b54d1f134cc07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EZANA001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecturer 001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lec001@ezana.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127001, localhost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79af36419cd79898533a2d9a3028c924fe0d720d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 Oct 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53c904468e7edec9a7f2501d8a8c8d5140c434cb</t>
+  </si>
   <si>
     <t xml:space="preserve">4085ff13746a078fc19d0f837fd02d35d3041291</t>
   </si>
@@ -34,18 +58,12 @@
     <t xml:space="preserve">lec002@ezana.org</t>
   </si>
   <si>
-    <t xml:space="preserve">127001, localhost</t>
-  </si>
-  <si>
     <t xml:space="preserve">a69681bcf334ae130217fea4505fd3c994f5683f</t>
   </si>
   <si>
     <t xml:space="preserve">1 Oct 2020</t>
   </si>
   <si>
-    <t xml:space="preserve">53c904468e7edec9a7f2501d8a8c8d5140c434cb</t>
-  </si>
-  <si>
     <t xml:space="preserve">4085ff13746a078fc19d0f837fd02d35d3041292</t>
   </si>
   <si>
@@ -365,9 +383,6 @@
   </si>
   <si>
     <t xml:space="preserve">127019, localhost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 Oct 2020</t>
   </si>
   <si>
     <t xml:space="preserve">4085ff13746a078fc19d0f837fd02d35d3041310</t>
@@ -608,10 +623,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -636,10 +651,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="n">
-        <v>3456787655</v>
+        <v>3456787654</v>
       </c>
       <c r="E1" s="0" t="n">
-        <v>23456789056</v>
+        <v>2548907654</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>3</v>
@@ -668,19 +683,19 @@
         <v>10</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>3456787656</v>
+        <v>3456787655</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>23456789057</v>
+        <v>23456789056</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>13</v>
@@ -700,10 +715,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>3456787657</v>
+        <v>3456787656</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>23456789058</v>
+        <v>23456789057</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>17</v>
@@ -712,7 +727,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>19</v>
@@ -732,10 +747,10 @@
         <v>22</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>3456787658</v>
+        <v>3456787657</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>23456789059</v>
+        <v>23456789058</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>23</v>
@@ -744,7 +759,7 @@
         <v>24</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>25</v>
@@ -764,10 +779,10 @@
         <v>28</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>3456787659</v>
+        <v>3456787658</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>23456789060</v>
+        <v>23456789059</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>29</v>
@@ -776,7 +791,7 @@
         <v>30</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>31</v>
@@ -796,10 +811,10 @@
         <v>34</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>3456787660</v>
+        <v>3456787659</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>23456789061</v>
+        <v>23456789060</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>35</v>
@@ -808,7 +823,7 @@
         <v>36</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>37</v>
@@ -828,10 +843,10 @@
         <v>40</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>3456787661</v>
+        <v>3456787660</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>23456789062</v>
+        <v>23456789061</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>41</v>
@@ -840,7 +855,7 @@
         <v>42</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>43</v>
@@ -860,10 +875,10 @@
         <v>46</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>3456787662</v>
+        <v>3456787661</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>23456789063</v>
+        <v>23456789062</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>47</v>
@@ -872,7 +887,7 @@
         <v>48</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>49</v>
@@ -892,10 +907,10 @@
         <v>52</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>3456787663</v>
+        <v>3456787662</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>23456789064</v>
+        <v>23456789063</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>53</v>
@@ -904,7 +919,7 @@
         <v>54</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>55</v>
@@ -924,10 +939,10 @@
         <v>58</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>3456787664</v>
+        <v>3456787663</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>23456789065</v>
+        <v>23456789064</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>59</v>
@@ -936,7 +951,7 @@
         <v>60</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>61</v>
@@ -956,10 +971,10 @@
         <v>64</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>3456787665</v>
+        <v>3456787664</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>23456789066</v>
+        <v>23456789065</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>65</v>
@@ -968,7 +983,7 @@
         <v>66</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>67</v>
@@ -988,10 +1003,10 @@
         <v>70</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>3456787666</v>
+        <v>3456787665</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>23456789067</v>
+        <v>23456789066</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>71</v>
@@ -1000,7 +1015,7 @@
         <v>72</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>73</v>
@@ -1020,10 +1035,10 @@
         <v>76</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>3456787667</v>
+        <v>3456787666</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>23456789068</v>
+        <v>23456789067</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>77</v>
@@ -1032,7 +1047,7 @@
         <v>78</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>79</v>
@@ -1052,10 +1067,10 @@
         <v>82</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>3456787668</v>
+        <v>3456787667</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>23456789069</v>
+        <v>23456789068</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>83</v>
@@ -1064,7 +1079,7 @@
         <v>84</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>85</v>
@@ -1084,10 +1099,10 @@
         <v>88</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>3456787669</v>
+        <v>3456787668</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>23456789070</v>
+        <v>23456789069</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>89</v>
@@ -1096,10 +1111,13 @@
         <v>90</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>91</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,10 +1131,10 @@
         <v>94</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>3456787670</v>
+        <v>3456787669</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>23456789071</v>
+        <v>23456789070</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>95</v>
@@ -1125,7 +1143,7 @@
         <v>96</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>97</v>
@@ -1142,10 +1160,10 @@
         <v>100</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>3456787671</v>
+        <v>3456787670</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>23456789072</v>
+        <v>23456789071</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>101</v>
@@ -1154,7 +1172,7 @@
         <v>102</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>103</v>
@@ -1171,10 +1189,10 @@
         <v>106</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>3456787672</v>
+        <v>3456787671</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>23456789073</v>
+        <v>23456789072</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>107</v>
@@ -1183,7 +1201,7 @@
         <v>108</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>109</v>
@@ -1200,10 +1218,10 @@
         <v>112</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>3456787673</v>
+        <v>3456787672</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>23456789074</v>
+        <v>23456789073</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>113</v>
@@ -1212,7 +1230,7 @@
         <v>114</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>115</v>
@@ -1229,10 +1247,10 @@
         <v>118</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>3456787674</v>
+        <v>3456787673</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>23456789075</v>
+        <v>23456789074</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>119</v>
@@ -1241,213 +1259,242 @@
         <v>120</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="0" t="n">
+        <v>3456787674</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>23456789075</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="D21" s="0" t="n">
-        <v>3456787675</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>23456789076</v>
-      </c>
-      <c r="F21" s="0" t="s">
+      <c r="G21" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="H21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="0" t="n">
+        <v>3456787675</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>23456789076</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="D22" s="0" t="n">
-        <v>3456787676</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>23456789077</v>
-      </c>
-      <c r="F22" s="0" t="s">
+      <c r="G22" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="H22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="C23" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="0" t="n">
+        <v>3456787676</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>23456789077</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="0" t="n">
-        <v>3456787677</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>23456789078</v>
-      </c>
-      <c r="F23" s="0" t="s">
+      <c r="G23" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="H23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="C24" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="D24" s="0" t="n">
+        <v>3456787677</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>23456789078</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D24" s="0" t="n">
-        <v>3456787678</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>23456789079</v>
-      </c>
-      <c r="F24" s="0" t="s">
+      <c r="G24" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="H24" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="C25" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" s="0" t="n">
+        <v>3456787678</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>23456789079</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="D25" s="0" t="n">
-        <v>3456787679</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>23456789080</v>
-      </c>
-      <c r="F25" s="0" t="s">
+      <c r="G25" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="H25" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="C26" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="D26" s="0" t="n">
+        <v>3456787679</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>23456789080</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="D26" s="0" t="n">
-        <v>3456787680</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>23456789081</v>
-      </c>
-      <c r="F26" s="0" t="s">
+      <c r="G26" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="H26" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="C27" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="D27" s="0" t="n">
+        <v>3456787680</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>23456789081</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="G27" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="0" t="n">
         <v>3456787681</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E28" s="0" t="n">
         <v>23456789082</v>
       </c>
-      <c r="F27" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>163</v>
+      <c r="F28" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>